<commit_message>
accessing username and password from excel sheet
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\B98_11AM_Selenium\Workspace\B98AFW\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharath P\git\B98AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BDD877D-89F6-4F17-A189-4B7B5CB13A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F10BA9-F2DE-42C9-AA48-D0DEA50C497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,9 +25,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>akshara</t>
+    <t>username</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>pointofsale</t>
   </si>
 </sst>
 </file>
@@ -345,17 +354,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Automation Script for InvalidLogin TC with test data
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharath P\git\B98AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F10BA9-F2DE-42C9-AA48-D0DEA50C497F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFE3E679-79C5-44A1-91A6-3878497239B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
+    <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -37,6 +38,12 @@
   </si>
   <si>
     <t>pointofsale</t>
+  </si>
+  <si>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -356,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -384,4 +391,39 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816BF25E-74DE-4A35-A5AF-565F3615FBD6}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Automation script for Create  New Supplier
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharath P\git\B98AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B17D558-B739-4E27-9FB6-EBCA16E6D289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DE5FE2-4249-41FB-8DBB-43A220512091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
     <sheet name="InvalidLogin" sheetId="2" r:id="rId2"/>
     <sheet name="PositionofSupplier" sheetId="3" r:id="rId3"/>
     <sheet name="VerifySupplierPage" sheetId="4" r:id="rId4"/>
+    <sheet name="CreateNewSupplier" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -46,6 +47,24 @@
   </si>
   <si>
     <t>xyz</t>
+  </si>
+  <si>
+    <t>companyname</t>
+  </si>
+  <si>
+    <t>firstname</t>
+  </si>
+  <si>
+    <t>lastname</t>
+  </si>
+  <si>
+    <t>parle</t>
+  </si>
+  <si>
+    <t>Prakash</t>
+  </si>
+  <si>
+    <t>Bhanu</t>
   </si>
 </sst>
 </file>
@@ -468,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6928B8F-B2CB-4A04-ACB5-11B06692DF1A}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -496,4 +515,56 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12006346-CA8C-44B7-8735-C7EDCB609369}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated CreateNewSupplier and DeleteASupplier tc
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sharath P\git\B98AFW\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3DE5FE2-4249-41FB-8DBB-43A220512091}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F487B1-AABA-405C-A412-F78254AC8F59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ValidLogin" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="PositionofSupplier" sheetId="3" r:id="rId3"/>
     <sheet name="VerifySupplierPage" sheetId="4" r:id="rId4"/>
     <sheet name="CreateNewSupplier" sheetId="5" r:id="rId5"/>
+    <sheet name="DeleteASupplier" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="12">
   <si>
     <t>username</t>
   </si>
@@ -521,7 +522,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12006346-CA8C-44B7-8735-C7EDCB609369}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
@@ -567,4 +568,38 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D34183FC-0A58-4928-AA0D-2A24E768CB1E}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O8" sqref="O8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>